<commit_message>
Tolto dalle espressioni il cast a Money
</commit_message>
<xml_diff>
--- a/BudgetHR/Local/License/Lyreco/Excel/Conti.xlsx
+++ b/BudgetHR/Local/License/Lyreco/Excel/Conti.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="19440" windowHeight="7995" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="19440" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Conti" sheetId="2" r:id="rId1"/>
@@ -134,63 +134,12 @@
     <t>Espressione Conto</t>
   </si>
   <si>
-    <t>Money(Sum(RAL))</t>
-  </si>
-  <si>
-    <t>Money(Sum([Retribuzione Lorda]))</t>
-  </si>
-  <si>
-    <t>Money(Sum(Bonus))</t>
-  </si>
-  <si>
-    <t>Money(Sum([Contributi su Retribuzione]))</t>
-  </si>
-  <si>
-    <t>Money(Sum(Straordinario))</t>
-  </si>
-  <si>
-    <t>Money(Sum([Contributi su Ratei]))</t>
-  </si>
-  <si>
-    <t>Money(Sum([Rateo 13ª Mensilità]))</t>
-  </si>
-  <si>
-    <t>Money(Sum([Rateo 14ª Mensilità]))</t>
-  </si>
-  <si>
-    <t>Money(Sum([Rateo Ferie e Festività]))</t>
-  </si>
-  <si>
-    <t>Money(Sum([Rateo TFR]))</t>
-  </si>
-  <si>
-    <t>Money(Sum([Rateo INAIL]))</t>
-  </si>
-  <si>
-    <t>Money(Sum([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket])</t>
-  </si>
-  <si>
-    <t>Money(Sum((Bonus / 13.5) - (Bonus * 0.005)))</t>
-  </si>
-  <si>
     <t>Sum([Ore Lavoro Ordinario])</t>
   </si>
   <si>
     <t>Sum([Ore Lavoro Straordinario])</t>
   </si>
   <si>
-    <t>Money(Sum(Aumento))</t>
-  </si>
-  <si>
-    <t>Money(Sum(Aumento) / 6)</t>
-  </si>
-  <si>
-    <t>Money(Sum([Aumento] * 0.0805864))</t>
-  </si>
-  <si>
-    <t>Money(Sum([Aumento] * [Rateo Ferie e Festività] / [RAL]))</t>
-  </si>
-  <si>
     <t>Maternità Retretribuzione Lorda + Ticket</t>
   </si>
   <si>
@@ -203,24 +152,247 @@
     <t>Maternità Contributi Straordinario</t>
   </si>
   <si>
-    <t>Money(Sum(
-  (Aumento 
-  + (Aumento / 6)
-  + ([Aumento] * [Rateo Ferie e Festività] / [RAL])
-  ) * [Aliquota Contributiva]
- ))</t>
-  </si>
-  <si>
-    <t>Money(Sum(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])))</t>
-  </si>
-  <si>
-    <t>Money(Sum(Bonus * [Aliquota Contributiva]))</t>
-  </si>
-  <si>
-    <t>Money(Sum(Straordinario * [Aliquota Contributiva]))</t>
-  </si>
-  <si>
-    <t>Money(Sum([Retribuzione Lorda])
+    <t>Maternità Facoltativa Retribuzione Lorda + Ticket</t>
+  </si>
+  <si>
+    <t>Maternità Facoltativa Straordinario</t>
+  </si>
+  <si>
+    <t>Maternità Facoltativa Rateo 13ª 14ª</t>
+  </si>
+  <si>
+    <t>Maternità Facoltativa Contributi Retribuzione Lorda + Ticket</t>
+  </si>
+  <si>
+    <t>Maternità Facoltativa Contributi Straordinario</t>
+  </si>
+  <si>
+    <t>Maternità Facoltativa Contributi Rateo 13ª 14ª + Ferie e Festività</t>
+  </si>
+  <si>
+    <t>Maternità Facoltativa Variabile/Bonus</t>
+  </si>
+  <si>
+    <t>Maternità Facoltativa Contributi su Variabile/Bonus</t>
+  </si>
+  <si>
+    <t>Maternità Facoltativa TFR su Variabile/Bonus</t>
+  </si>
+  <si>
+    <t>Maternità Facoltativa Rateo INAIL</t>
+  </si>
+  <si>
+    <t>Cessato Rateo 13ª 14ª Mensilità</t>
+  </si>
+  <si>
+    <t>Cessato Retribuzione Lorda + Ticket</t>
+  </si>
+  <si>
+    <t>Cessato Straordinario</t>
+  </si>
+  <si>
+    <t>Cessato Facoltativa Rateo INAIL</t>
+  </si>
+  <si>
+    <t>Cessato Contributi su Straordinario</t>
+  </si>
+  <si>
+    <t>Cessato Contributi Retribuzione Lorda + Ticket</t>
+  </si>
+  <si>
+    <t>Più di 5 mesi di Maternità</t>
+  </si>
+  <si>
+    <t>Maternità con valore diverso da 0 o 1</t>
+  </si>
+  <si>
+    <t>Maternità Facoltativa con valore diverso da 0 o 1</t>
+  </si>
+  <si>
+    <t>Cessato con valore diverso da 0 o 1</t>
+  </si>
+  <si>
+    <t>ExpressionID</t>
+  </si>
+  <si>
+    <t>Alert</t>
+  </si>
+  <si>
+    <t>Expression</t>
+  </si>
+  <si>
+    <t>Count({&lt;[Maternità]=E({&lt;[Maternità]={0,1}&gt;}) &gt;} DISTINCT [Maternità]) &gt; 0</t>
+  </si>
+  <si>
+    <t>Count({&lt;[Cessato]=E({&lt;[Cessato]={0,1}&gt;}) &gt;} DISTINCT [Cessato]) &gt; 0</t>
+  </si>
+  <si>
+    <t>Dipendente Cessato, Aumento non ammesso</t>
+  </si>
+  <si>
+    <t>Dipendente Cessato, Maternità non ammessa</t>
+  </si>
+  <si>
+    <t>Dipendente Cessato, Maternità Facoltativa non ammessa</t>
+  </si>
+  <si>
+    <t>Dipendente Cessato, Ferie non ammesse</t>
+  </si>
+  <si>
+    <t>Ferie Godute può asumere solo valori &gt;= 0</t>
+  </si>
+  <si>
+    <t>Count({&lt;[Ferie Godute]={'&lt;0'}&gt;} DISTINCT [Ferie Godute]) &gt; 0</t>
+  </si>
+  <si>
+    <t>Count({&lt;[Cessato]={1}, [Aumento]=E({&lt;[Aumento]={0}&gt;}) &gt;} DISTINCT [Cessato]) &gt; 0</t>
+  </si>
+  <si>
+    <t>Count({&lt;[Cessato]={1}, [Maternità]=E({&lt;[Maternità]={0}&gt;}) &gt;} DISTINCT [Cessato]) &gt; 0</t>
+  </si>
+  <si>
+    <t>Count({&lt;[Cessato]={1}, [Maternità Facoltativa]=E({&lt;[Maternità Facoltativa]={0}&gt;}) &gt;} DISTINCT [Cessato]) &gt; 0</t>
+  </si>
+  <si>
+    <t>Count({&lt;[Cessato]={1}, [Ferie Godute]=E({&lt;[Ferie Godute]={0}&gt;}) &gt;} DISTINCT [Cessato]) &gt; 0</t>
+  </si>
+  <si>
+    <t>Count({&lt;[Maternità Facoltativa]=E({&lt;[Maternità Facoltativa]={0,1}&gt;}) &gt;} DISTINCT [Maternità Facoltativa]) &gt; 0</t>
+  </si>
+  <si>
+    <t>Count({&lt;[Cessato]={1}, [Straordinario]=E({&lt;[Straordinario]={0}&gt;}) &gt;} DISTINCT [Cessato]) &gt; 0</t>
+  </si>
+  <si>
+    <t>Count({&lt;[Cessato]={1}, [Bonus]=E({&lt;[Bonus]={0}&gt;}) &gt;} DISTINCT [Cessato]) &gt; 0</t>
+  </si>
+  <si>
+    <t>Dipendente Cessato, Straordinario non ammesso</t>
+  </si>
+  <si>
+    <t>Dipendente Cessato, Bonus non ammesso</t>
+  </si>
+  <si>
+    <t>Maternità e Ferie Godute presenti sullo stesso mese</t>
+  </si>
+  <si>
+    <t>Maternità e Maternità Facoltativa presenti sullo stesso mese</t>
+  </si>
+  <si>
+    <t>Maternità Facoltativa e Ferie Godute presenti sullo stesso mese</t>
+  </si>
+  <si>
+    <t>Maternità, Maternità Facoltativa e Ferie Godute presenti sullo stesso mese</t>
+  </si>
+  <si>
+    <t>Count({&lt;[Maternità]={1}, [Maternità Facoltativa]={1}&gt;} DISTINCT [Maternità]) &gt; 0</t>
+  </si>
+  <si>
+    <t>Count({&lt;[Maternità]={1}, [Ferie Godute]={'&gt;0'}&gt;} DISTINCT [Maternità]) &gt; 0</t>
+  </si>
+  <si>
+    <t>Count({&lt;[Maternità Facoltativa]={1}, [Ferie Godute]={'&gt;0'}&gt;} DISTINCT [Maternità Facoltativa]) &gt; 0</t>
+  </si>
+  <si>
+    <t>Count({&lt;[Maternità]={1}, [Maternità Facoltativa]={1}, [Ferie Godute]={'&gt;0'}&gt;} DISTINCT [Maternità]) &gt; 0</t>
+  </si>
+  <si>
+    <t>Sum(Aggr(Count({&lt;Maternità={1}&gt;} DISTINCT Maternità), Key_Azienda_Filiale_Matricola)) &gt; 5</t>
+  </si>
+  <si>
+    <t>Ore Lavoro Straordinario Variazione</t>
+  </si>
+  <si>
+    <t>Num(Sum([Straordinario] / (([RAL] / 168) * [Maggiorazione Straordinario])), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Ferie Godute Quantità</t>
+  </si>
+  <si>
+    <t>Num(Sum([Ferie Godute]), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>N.A.002</t>
+  </si>
+  <si>
+    <t>N.A.003</t>
+  </si>
+  <si>
+    <t>N.A.004</t>
+  </si>
+  <si>
+    <t>N.A.005</t>
+  </si>
+  <si>
+    <t>N.A.006</t>
+  </si>
+  <si>
+    <t>N.A.007</t>
+  </si>
+  <si>
+    <t>N.A.008</t>
+  </si>
+  <si>
+    <t>N.A.001</t>
+  </si>
+  <si>
+    <t>Dipendente Cessato, Bonus non spettante perché i giorni lavorati nell'anno sono &lt;= 180</t>
+  </si>
+  <si>
+    <t>(Sum({&lt;[Bonus]=E({&lt;[Bonus]={0}&gt;})&gt;} TOTAL&lt;[Ragione Sociale], [Matricola - Dipendente]&gt; 
+   Aggr(Min({&lt;Cessato={1}&gt;} TOTAL&lt;Key_Azienda_Filiale_Matricola&gt; Data) - 
+   RangeMax([Data Assunzione], MakeDate(Year(Today()) + 1)), Key_Azienda_Filiale_Matricola)) &lt;= 180
+   AND Count({&lt;[Cessato]={1}, [Bonus]=E({&lt;[Bonus]={0}&gt;}) &gt;} TOTAL&lt;[Ragione Sociale], [Matricola - Dipendente]&gt; DISTINCT [Cessato]) &gt; 0)</t>
+  </si>
+  <si>
+    <t>(Sum(RAL))</t>
+  </si>
+  <si>
+    <t>(Sum([Retribuzione Lorda]))</t>
+  </si>
+  <si>
+    <t>(Sum([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket])</t>
+  </si>
+  <si>
+    <t>(Sum(Bonus))</t>
+  </si>
+  <si>
+    <t>(Sum(Straordinario))</t>
+  </si>
+  <si>
+    <t>(Sum([Contributi su Retribuzione]))</t>
+  </si>
+  <si>
+    <t>(Sum(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])))</t>
+  </si>
+  <si>
+    <t>(Sum(Bonus * [Aliquota Contributiva]))</t>
+  </si>
+  <si>
+    <t>(Sum(Straordinario * [Aliquota Contributiva]))</t>
+  </si>
+  <si>
+    <t>(Sum([Rateo 13ª Mensilità]))</t>
+  </si>
+  <si>
+    <t>(Sum([Rateo 14ª Mensilità]))</t>
+  </si>
+  <si>
+    <t>(Sum([Rateo Ferie e Festività]))</t>
+  </si>
+  <si>
+    <t>(Sum([Rateo TFR]))</t>
+  </si>
+  <si>
+    <t>(Sum((Bonus / 13.5) - (Bonus * 0.005)))</t>
+  </si>
+  <si>
+    <t>(Sum([Rateo INAIL]))</t>
+  </si>
+  <si>
+    <t>(Sum([Contributi su Ratei]))</t>
+  </si>
+  <si>
+    <t>(Sum([Retribuzione Lorda])
   + Sum([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]
   + Sum(Bonus)
   + Sum(Straordinario)
@@ -238,238 +410,7 @@
  )</t>
   </si>
   <si>
-    <t>Maternità Facoltativa Retribuzione Lorda + Ticket</t>
-  </si>
-  <si>
-    <t>Maternità Facoltativa Straordinario</t>
-  </si>
-  <si>
-    <t>Maternità Facoltativa Rateo 13ª 14ª</t>
-  </si>
-  <si>
-    <t>Maternità Facoltativa Contributi Retribuzione Lorda + Ticket</t>
-  </si>
-  <si>
-    <t>Maternità Facoltativa Contributi Straordinario</t>
-  </si>
-  <si>
-    <t>Maternità Facoltativa Contributi Rateo 13ª 14ª + Ferie e Festività</t>
-  </si>
-  <si>
-    <t>Maternità Facoltativa Variabile/Bonus</t>
-  </si>
-  <si>
-    <t>Maternità Facoltativa Contributi su Variabile/Bonus</t>
-  </si>
-  <si>
-    <t>Maternità Facoltativa TFR su Variabile/Bonus</t>
-  </si>
-  <si>
-    <t>Maternità Facoltativa Rateo INAIL</t>
-  </si>
-  <si>
-    <t>Money(Sum(-[RAL] / 26 * [Ferie Godute]))</t>
-  </si>
-  <si>
-    <t>Money(Sum(-[RAL] / 26 * [Ferie Godute] * [Aliquota Contributiva]))</t>
-  </si>
-  <si>
-    <t>Cessato Rateo 13ª 14ª Mensilità</t>
-  </si>
-  <si>
-    <t>Money(Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità])) * [Cessato])</t>
-  </si>
-  <si>
-    <t>Money(Sum(-[Rateo Ferie e Festività]) * [Cessato])</t>
-  </si>
-  <si>
-    <t>Money(Sum(-Bonus) * [Cessato])</t>
-  </si>
-  <si>
-    <t>Money(Sum(-Bonus * [Aliquota Contributiva]) * [Cessato])</t>
-  </si>
-  <si>
-    <t>Money(Sum((-Bonus / 13.5) - (-Bonus * 0.005)) * [Cessato])</t>
-  </si>
-  <si>
-    <t>Money(Sum(-[Contributi su Ratei]) * [Cessato])</t>
-  </si>
-  <si>
-    <t>Money(Sum(-[Rateo TFR]) * [Cessato])</t>
-  </si>
-  <si>
-    <t>Money(Sum(RangeSum(-[Retribuzione Lorda] , -(([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]))) * [Cessato])</t>
-  </si>
-  <si>
-    <t>Cessato Retribuzione Lorda + Ticket</t>
-  </si>
-  <si>
-    <t>Money(Sum(-Straordinario) * [Cessato])</t>
-  </si>
-  <si>
-    <t>Cessato Straordinario</t>
-  </si>
-  <si>
-    <t>Cessato Facoltativa Rateo INAIL</t>
-  </si>
-  <si>
-    <t>Money(Sum(-[Rateo INAIL]) * [Cessato])</t>
-  </si>
-  <si>
-    <t>Cessato Contributi su Straordinario</t>
-  </si>
-  <si>
-    <t>Cessato Contributi Retribuzione Lorda + Ticket</t>
-  </si>
-  <si>
-    <t>Money(Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])))) * [Cessato])</t>
-  </si>
-  <si>
-    <t>Più di 5 mesi di Maternità</t>
-  </si>
-  <si>
-    <t>Maternità con valore diverso da 0 o 1</t>
-  </si>
-  <si>
-    <t>Maternità Facoltativa con valore diverso da 0 o 1</t>
-  </si>
-  <si>
-    <t>Cessato con valore diverso da 0 o 1</t>
-  </si>
-  <si>
-    <t>ExpressionID</t>
-  </si>
-  <si>
-    <t>Alert</t>
-  </si>
-  <si>
-    <t>Expression</t>
-  </si>
-  <si>
-    <t>Count({&lt;[Maternità]=E({&lt;[Maternità]={0,1}&gt;}) &gt;} DISTINCT [Maternità]) &gt; 0</t>
-  </si>
-  <si>
-    <t>Count({&lt;[Cessato]=E({&lt;[Cessato]={0,1}&gt;}) &gt;} DISTINCT [Cessato]) &gt; 0</t>
-  </si>
-  <si>
-    <t>Dipendente Cessato, Aumento non ammesso</t>
-  </si>
-  <si>
-    <t>Dipendente Cessato, Maternità non ammessa</t>
-  </si>
-  <si>
-    <t>Dipendente Cessato, Maternità Facoltativa non ammessa</t>
-  </si>
-  <si>
-    <t>Dipendente Cessato, Ferie non ammesse</t>
-  </si>
-  <si>
-    <t>Ferie Godute può asumere solo valori &gt;= 0</t>
-  </si>
-  <si>
-    <t>Count({&lt;[Ferie Godute]={'&lt;0'}&gt;} DISTINCT [Ferie Godute]) &gt; 0</t>
-  </si>
-  <si>
-    <t>Count({&lt;[Cessato]={1}, [Aumento]=E({&lt;[Aumento]={0}&gt;}) &gt;} DISTINCT [Cessato]) &gt; 0</t>
-  </si>
-  <si>
-    <t>Count({&lt;[Cessato]={1}, [Maternità]=E({&lt;[Maternità]={0}&gt;}) &gt;} DISTINCT [Cessato]) &gt; 0</t>
-  </si>
-  <si>
-    <t>Count({&lt;[Cessato]={1}, [Maternità Facoltativa]=E({&lt;[Maternità Facoltativa]={0}&gt;}) &gt;} DISTINCT [Cessato]) &gt; 0</t>
-  </si>
-  <si>
-    <t>Count({&lt;[Cessato]={1}, [Ferie Godute]=E({&lt;[Ferie Godute]={0}&gt;}) &gt;} DISTINCT [Cessato]) &gt; 0</t>
-  </si>
-  <si>
-    <t>Count({&lt;[Maternità Facoltativa]=E({&lt;[Maternità Facoltativa]={0,1}&gt;}) &gt;} DISTINCT [Maternità Facoltativa]) &gt; 0</t>
-  </si>
-  <si>
-    <t>Money(Sum(RangeSum(-[Retribuzione Lorda] , -(([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]))) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>Money(Sum(-Straordinario) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>Money(Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità])) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>Money(Sum(-[Rateo Ferie e Festività]) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>Money(Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])))) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>Money(Sum(-Straordinario * [Aliquota Contributiva]) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>Money(Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità], -[Rateo Ferie e Festività]) * [Aliquota Contributiva]) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>Money(Sum(-Bonus) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>Money(Sum(-Bonus * [Aliquota Contributiva]) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>Money(Sum((-Bonus / 13.5) - (-Bonus * 0.005)) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>Money(Sum(-[Rateo INAIL]) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>Count({&lt;[Cessato]={1}, [Straordinario]=E({&lt;[Straordinario]={0}&gt;}) &gt;} DISTINCT [Cessato]) &gt; 0</t>
-  </si>
-  <si>
-    <t>Count({&lt;[Cessato]={1}, [Bonus]=E({&lt;[Bonus]={0}&gt;}) &gt;} DISTINCT [Cessato]) &gt; 0</t>
-  </si>
-  <si>
-    <t>Dipendente Cessato, Straordinario non ammesso</t>
-  </si>
-  <si>
-    <t>Dipendente Cessato, Bonus non ammesso</t>
-  </si>
-  <si>
-    <t>Maternità e Ferie Godute presenti sullo stesso mese</t>
-  </si>
-  <si>
-    <t>Maternità e Maternità Facoltativa presenti sullo stesso mese</t>
-  </si>
-  <si>
-    <t>Maternità Facoltativa e Ferie Godute presenti sullo stesso mese</t>
-  </si>
-  <si>
-    <t>Maternità, Maternità Facoltativa e Ferie Godute presenti sullo stesso mese</t>
-  </si>
-  <si>
-    <t>Count({&lt;[Maternità]={1}, [Maternità Facoltativa]={1}&gt;} DISTINCT [Maternità]) &gt; 0</t>
-  </si>
-  <si>
-    <t>Count({&lt;[Maternità]={1}, [Ferie Godute]={'&gt;0'}&gt;} DISTINCT [Maternità]) &gt; 0</t>
-  </si>
-  <si>
-    <t>Count({&lt;[Maternità Facoltativa]={1}, [Ferie Godute]={'&gt;0'}&gt;} DISTINCT [Maternità Facoltativa]) &gt; 0</t>
-  </si>
-  <si>
-    <t>Count({&lt;[Maternità]={1}, [Maternità Facoltativa]={1}, [Ferie Godute]={'&gt;0'}&gt;} DISTINCT [Maternità]) &gt; 0</t>
-  </si>
-  <si>
-    <t>Sum(Aggr(Count({&lt;Maternità={1}&gt;} DISTINCT Maternità), Key_Azienda_Filiale_Matricola)) &gt; 5</t>
-  </si>
-  <si>
-    <t>Ore Lavoro Straordinario Variazione</t>
-  </si>
-  <si>
-    <t>Num(Sum([Straordinario] / (([RAL] / 168) * [Maggiorazione Straordinario])), '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Ferie Godute Quantità</t>
-  </si>
-  <si>
-    <t>Num(Sum([Ferie Godute]), '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Money((Sum([Retribuzione Lorda])
+    <t>((Sum([Retribuzione Lorda])
   + Sum([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]
   + Sum(Bonus)
   + Sum(Straordinario)
@@ -487,10 +428,117 @@
   ) / (Sum([Ore Lavoro Ordinario]) + Sum([Ore Lavoro Straordinario]) + Sum([Straordinario] / (([RAL] / 168) * [Maggiorazione Straordinario]))))</t>
   </si>
   <si>
-    <t>Money(Sum(-Straordinario * [Aliquota Contributiva])* [Cessato])</t>
-  </si>
-  <si>
-    <t>Money(Sum([Retribuzione Lorda])
+    <t>(Sum(Aumento))</t>
+  </si>
+  <si>
+    <t>(Sum(Aumento) / 6)</t>
+  </si>
+  <si>
+    <t>(Sum([Aumento] * [Rateo Ferie e Festività] / [RAL]))</t>
+  </si>
+  <si>
+    <t>(Sum([Aumento] * 0.0805864))</t>
+  </si>
+  <si>
+    <t>(Sum(
+  (Aumento 
+  + (Aumento / 6)
+  + ([Aumento] * [Rateo Ferie e Festività] / [RAL])
+  ) * [Aliquota Contributiva]
+ ))</t>
+  </si>
+  <si>
+    <t>(Sum(RangeSum(-([RAL] * 0.8), - (([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]))) * Alt([Maternità], 0))</t>
+  </si>
+  <si>
+    <t>(Sum(-Straordinario) * Alt([Maternità], 0))</t>
+  </si>
+  <si>
+    <t>(Sum(RangeSum(
+ - ([RAL] * 0.8 * [Aliquota Contributiva])
+ - ((([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])))
+)) * Alt([Maternità], 0))</t>
+  </si>
+  <si>
+    <t>(Sum(-Straordinario * [Aliquota Contributiva]) * Alt([Maternità], 0))</t>
+  </si>
+  <si>
+    <t>(Sum(RangeSum(-[Retribuzione Lorda] , -(([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]))) * [Maternità Facoltativa])</t>
+  </si>
+  <si>
+    <t>(Sum(-Straordinario) * [Maternità Facoltativa])</t>
+  </si>
+  <si>
+    <t>(Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità])) * [Maternità Facoltativa])</t>
+  </si>
+  <si>
+    <t>(Sum(-[Rateo Ferie e Festività]) * [Maternità Facoltativa])</t>
+  </si>
+  <si>
+    <t>(Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])))) * [Maternità Facoltativa])</t>
+  </si>
+  <si>
+    <t>(Sum(-Straordinario * [Aliquota Contributiva]) * [Maternità Facoltativa])</t>
+  </si>
+  <si>
+    <t>(Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità], -[Rateo Ferie e Festività]) * [Aliquota Contributiva]) * [Maternità Facoltativa])</t>
+  </si>
+  <si>
+    <t>(Sum(-Bonus) * [Maternità Facoltativa])</t>
+  </si>
+  <si>
+    <t>(Sum(-Bonus * [Aliquota Contributiva]) * [Maternità Facoltativa])</t>
+  </si>
+  <si>
+    <t>(Sum((-Bonus / 13.5) - (-Bonus * 0.005)) * [Maternità Facoltativa])</t>
+  </si>
+  <si>
+    <t>(Sum(-[Rateo INAIL]) * [Maternità Facoltativa])</t>
+  </si>
+  <si>
+    <t>(Sum(-[RAL] / 26 * [Ferie Godute]))</t>
+  </si>
+  <si>
+    <t>(Sum(-[RAL] / 26 * [Ferie Godute] * [Aliquota Contributiva]))</t>
+  </si>
+  <si>
+    <t>(Sum(RangeSum(-[Retribuzione Lorda] , -(([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]))) * [Cessato])</t>
+  </si>
+  <si>
+    <t>(Sum(-Straordinario) * [Cessato])</t>
+  </si>
+  <si>
+    <t>(Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità])) * [Cessato])</t>
+  </si>
+  <si>
+    <t>(Sum(-[Rateo Ferie e Festività]) * [Cessato])</t>
+  </si>
+  <si>
+    <t>(Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])))) * [Cessato])</t>
+  </si>
+  <si>
+    <t>(Sum(-Straordinario * [Aliquota Contributiva])* [Cessato])</t>
+  </si>
+  <si>
+    <t>(Sum(-Bonus) * [Cessato])</t>
+  </si>
+  <si>
+    <t>(Sum(-Bonus * [Aliquota Contributiva]) * [Cessato])</t>
+  </si>
+  <si>
+    <t>(Sum((-Bonus / 13.5) - (-Bonus * 0.005)) * [Cessato])</t>
+  </si>
+  <si>
+    <t>(Sum(-[Contributi su Ratei]) * [Cessato])</t>
+  </si>
+  <si>
+    <t>(Sum(-[Rateo TFR]) * [Cessato])</t>
+  </si>
+  <si>
+    <t>(Sum(-[Rateo INAIL]) * [Cessato])</t>
+  </si>
+  <si>
+    <t>(Sum([Retribuzione Lorda])
   + Sum([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]
   + Sum(Bonus)
   + Sum(Straordinario)
@@ -548,54 +596,6 @@
   + (Sum(-[Rateo TFR]) * [Cessato])
   + (Sum(-[Rateo INAIL]) * [Cessato])
  )</t>
-  </si>
-  <si>
-    <t>Money(Sum(RangeSum(-([RAL] * 0.8), - (([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]))) * Alt([Maternità], 0))</t>
-  </si>
-  <si>
-    <t>Money(Sum(-Straordinario) * Alt([Maternità], 0))</t>
-  </si>
-  <si>
-    <t>Money(Sum(RangeSum(
- - ([RAL] * 0.8 * [Aliquota Contributiva])
- - ((([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])))
-)) * Alt([Maternità], 0))</t>
-  </si>
-  <si>
-    <t>Money(Sum(-Straordinario * [Aliquota Contributiva]) * Alt([Maternità], 0))</t>
-  </si>
-  <si>
-    <t>N.A.002</t>
-  </si>
-  <si>
-    <t>N.A.003</t>
-  </si>
-  <si>
-    <t>N.A.004</t>
-  </si>
-  <si>
-    <t>N.A.005</t>
-  </si>
-  <si>
-    <t>N.A.006</t>
-  </si>
-  <si>
-    <t>N.A.007</t>
-  </si>
-  <si>
-    <t>N.A.008</t>
-  </si>
-  <si>
-    <t>N.A.001</t>
-  </si>
-  <si>
-    <t>Dipendente Cessato, Bonus non spettante perché i giorni lavorati nell'anno sono &lt;= 180</t>
-  </si>
-  <si>
-    <t>(Sum({&lt;[Bonus]=E({&lt;[Bonus]={0}&gt;})&gt;} TOTAL&lt;[Ragione Sociale], [Matricola - Dipendente]&gt; 
-   Aggr(Min({&lt;Cessato={1}&gt;} TOTAL&lt;Key_Azienda_Filiale_Matricola&gt; Data) - 
-   RangeMax([Data Assunzione], MakeDate(Year(Today()) + 1)), Key_Azienda_Filiale_Matricola)) &lt;= 180
-   AND Count({&lt;[Cessato]={1}, [Bonus]=E({&lt;[Bonus]={0}&gt;}) &gt;} TOTAL&lt;[Ragione Sociale], [Matricola - Dipendente]&gt; DISTINCT [Cessato]) &gt; 0)</t>
   </si>
 </sst>
 </file>
@@ -665,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -697,6 +697,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -994,30 +997,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="96.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="128.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="12" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1026,13 +1029,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>158</v>
+        <v>105</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1046,7 +1049,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>40</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1060,7 +1063,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1074,7 +1077,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>41</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1088,7 +1091,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1102,7 +1105,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>42</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1116,7 +1119,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>63</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1130,7 +1133,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>64</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1144,7 +1147,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1158,7 +1161,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1172,7 +1175,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>46</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1186,7 +1189,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>47</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1200,7 +1203,7 @@
         <v>4</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>48</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1214,7 +1217,7 @@
         <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1228,7 +1231,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>49</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1242,7 +1245,7 @@
         <v>16</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>44</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="60" customHeight="1">
@@ -1250,13 +1253,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>151</v>
+        <v>98</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>66</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1264,13 +1267,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>152</v>
+        <v>99</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1278,13 +1281,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>153</v>
+        <v>100</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1292,13 +1295,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>154</v>
+        <v>101</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>140</v>
+        <v>94</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>141</v>
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="76.5" customHeight="1">
@@ -1306,13 +1309,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>155</v>
+        <v>102</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>144</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1326,7 +1329,7 @@
         <v>21</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>54</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1340,7 +1343,7 @@
         <v>22</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1354,7 +1357,7 @@
         <v>23</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1368,7 +1371,7 @@
         <v>24</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>56</v>
+        <v>129</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="72">
@@ -1382,7 +1385,7 @@
         <v>25</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>62</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1393,10 +1396,10 @@
         <v>140001</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1407,10 +1410,10 @@
         <v>140301</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="48">
@@ -1421,10 +1424,10 @@
         <v>143001</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1435,10 +1438,10 @@
         <v>143001</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1449,10 +1452,10 @@
         <v>140001</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1463,10 +1466,10 @@
         <v>140301</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1477,10 +1480,10 @@
         <v>140003</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1494,7 +1497,7 @@
         <v>29</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>119</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1505,10 +1508,10 @@
         <v>143001</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>120</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1519,10 +1522,10 @@
         <v>143001</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1533,10 +1536,10 @@
         <v>143012</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1547,10 +1550,10 @@
         <v>140201</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1561,10 +1564,10 @@
         <v>143001</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1575,10 +1578,10 @@
         <v>140402</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1589,10 +1592,10 @@
         <v>143002</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>126</v>
+        <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1600,13 +1603,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>156</v>
+        <v>103</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>142</v>
+        <v>96</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>143</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:4">
@@ -1620,7 +1623,7 @@
         <v>30</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>77</v>
+        <v>146</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1634,7 +1637,7 @@
         <v>31</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>78</v>
+        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1645,10 +1648,10 @@
         <v>140001</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>87</v>
+        <v>148</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1659,10 +1662,10 @@
         <v>140301</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>90</v>
+        <v>57</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>89</v>
+        <v>149</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1673,10 +1676,10 @@
         <v>140003</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>80</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1690,7 +1693,7 @@
         <v>32</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>81</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1701,10 +1704,10 @@
         <v>143001</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>95</v>
+        <v>152</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1715,10 +1718,10 @@
         <v>143001</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1732,7 +1735,7 @@
         <v>33</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>82</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1746,7 +1749,7 @@
         <v>35</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>83</v>
+        <v>155</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1760,7 +1763,7 @@
         <v>37</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>84</v>
+        <v>156</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1774,7 +1777,7 @@
         <v>34</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>85</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1788,7 +1791,7 @@
         <v>36</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>86</v>
+        <v>158</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1799,10 +1802,10 @@
         <v>143002</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>91</v>
+        <v>58</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>92</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="99.95" customHeight="1">
@@ -1810,13 +1813,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>157</v>
+        <v>104</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>146</v>
+        <v>160</v>
       </c>
       <c r="E58" s="4"/>
     </row>
@@ -1830,7 +1833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1844,13 +1847,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="9" t="s">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1858,10 +1861,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>96</v>
+        <v>61</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>139</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1869,10 +1872,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>97</v>
+        <v>62</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1880,10 +1883,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>98</v>
+        <v>63</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1891,10 +1894,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>99</v>
+        <v>64</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1902,10 +1905,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>111</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1913,10 +1916,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>129</v>
+        <v>83</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>127</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1924,10 +1927,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>130</v>
+        <v>84</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>128</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="60">
@@ -1935,10 +1938,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>159</v>
+        <v>106</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>160</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1946,10 +1949,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1957,10 +1960,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1968,10 +1971,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1979,10 +1982,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1990,10 +1993,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>132</v>
+        <v>86</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>135</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2001,10 +2004,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>136</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2012,10 +2015,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>133</v>
+        <v>87</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>137</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2023,10 +2026,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>134</v>
+        <v>88</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>138</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiunto cast a Num al mosto di Money
</commit_message>
<xml_diff>
--- a/BudgetHR/Local/License/Lyreco/Excel/Conti.xlsx
+++ b/BudgetHR/Local/License/Lyreco/Excel/Conti.xlsx
@@ -344,55 +344,55 @@
    AND Count({&lt;[Cessato]={1}, [Bonus]=E({&lt;[Bonus]={0}&gt;}) &gt;} TOTAL&lt;[Ragione Sociale], [Matricola - Dipendente]&gt; DISTINCT [Cessato]) &gt; 0)</t>
   </si>
   <si>
-    <t>(Sum(RAL))</t>
-  </si>
-  <si>
-    <t>(Sum([Retribuzione Lorda]))</t>
-  </si>
-  <si>
-    <t>(Sum([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket])</t>
-  </si>
-  <si>
-    <t>(Sum(Bonus))</t>
-  </si>
-  <si>
-    <t>(Sum(Straordinario))</t>
-  </si>
-  <si>
-    <t>(Sum([Contributi su Retribuzione]))</t>
-  </si>
-  <si>
-    <t>(Sum(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])))</t>
-  </si>
-  <si>
-    <t>(Sum(Bonus * [Aliquota Contributiva]))</t>
-  </si>
-  <si>
-    <t>(Sum(Straordinario * [Aliquota Contributiva]))</t>
-  </si>
-  <si>
-    <t>(Sum([Rateo 13ª Mensilità]))</t>
-  </si>
-  <si>
-    <t>(Sum([Rateo 14ª Mensilità]))</t>
-  </si>
-  <si>
-    <t>(Sum([Rateo Ferie e Festività]))</t>
-  </si>
-  <si>
-    <t>(Sum([Rateo TFR]))</t>
-  </si>
-  <si>
-    <t>(Sum((Bonus / 13.5) - (Bonus * 0.005)))</t>
-  </si>
-  <si>
-    <t>(Sum([Rateo INAIL]))</t>
-  </si>
-  <si>
-    <t>(Sum([Contributi su Ratei]))</t>
-  </si>
-  <si>
-    <t>(Sum([Retribuzione Lorda])
+    <t>Num(Sum(Straordinario))</t>
+  </si>
+  <si>
+    <t>Num(Sum(RAL), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum([Retribuzione Lorda]), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(Bonus), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum([Contributi su Retribuzione]), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(Bonus * [Aliquota Contributiva]), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(Straordinario * [Aliquota Contributiva]), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum([Rateo 13ª Mensilità]), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum([Rateo 14ª Mensilità]), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum([Rateo Ferie e Festività]), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum([Rateo TFR]), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum((Bonus / 13.5) - (Bonus * 0.005)), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum([Rateo INAIL]), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum([Contributi su Ratei]), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num((Sum([Retribuzione Lorda])
   + Sum([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]
   + Sum(Bonus)
   + Sum(Straordinario)
@@ -407,138 +407,120 @@
   + Sum((Bonus / 13.5) - (Bonus * 0.005))
   + Sum([Rateo INAIL])
   + Sum([Contributi su Ratei])
- )</t>
-  </si>
-  <si>
-    <t>((Sum([Retribuzione Lorda])
-  + Sum([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]
-  + Sum(Bonus)
-  + Sum(Straordinario)
-  + Sum([Contributi su Retribuzione])
-  + Sum(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva]))
-  + Sum(Bonus * [Aliquota Contributiva])
-  + Sum(Straordinario * [Aliquota Contributiva])
-  + Sum([Rateo 13ª Mensilità])
-  + Sum([Rateo 14ª Mensilità])
-  + Sum([Rateo Ferie e Festività])
-  + Sum([Rateo TFR])
-  + Sum((Bonus / 13.5) - (Bonus * 0.005))
-  + Sum([Rateo INAIL])
-  + Sum([Contributi su Ratei])
-  ) / (Sum([Ore Lavoro Ordinario]) + Sum([Ore Lavoro Straordinario]) + Sum([Straordinario] / (([RAL] / 168) * [Maggiorazione Straordinario]))))</t>
-  </si>
-  <si>
-    <t>(Sum(Aumento))</t>
-  </si>
-  <si>
-    <t>(Sum(Aumento) / 6)</t>
-  </si>
-  <si>
-    <t>(Sum([Aumento] * [Rateo Ferie e Festività] / [RAL]))</t>
-  </si>
-  <si>
-    <t>(Sum([Aumento] * 0.0805864))</t>
-  </si>
-  <si>
-    <t>(Sum(
+  ) / (Sum([Ore Lavoro Ordinario]) + Sum([Ore Lavoro Straordinario]) + Sum([Straordinario] / (([RAL] / 168) * [Maggiorazione Straordinario]))), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(
   (Aumento 
   + (Aumento / 6)
   + ([Aumento] * [Rateo Ferie e Festività] / [RAL])
   ) * [Aliquota Contributiva]
- ))</t>
-  </si>
-  <si>
-    <t>(Sum(RangeSum(-([RAL] * 0.8), - (([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]))) * Alt([Maternità], 0))</t>
-  </si>
-  <si>
-    <t>(Sum(-Straordinario) * Alt([Maternità], 0))</t>
-  </si>
-  <si>
-    <t>(Sum(RangeSum(
+ ), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(RangeSum(
  - ([RAL] * 0.8 * [Aliquota Contributiva])
  - ((([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])))
-)) * Alt([Maternità], 0))</t>
-  </si>
-  <si>
-    <t>(Sum(-Straordinario * [Aliquota Contributiva]) * Alt([Maternità], 0))</t>
-  </si>
-  <si>
-    <t>(Sum(RangeSum(-[Retribuzione Lorda] , -(([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]))) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>(Sum(-Straordinario) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>(Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità])) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>(Sum(-[Rateo Ferie e Festività]) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>(Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])))) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>(Sum(-Straordinario * [Aliquota Contributiva]) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>(Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità], -[Rateo Ferie e Festività]) * [Aliquota Contributiva]) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>(Sum(-Bonus) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>(Sum(-Bonus * [Aliquota Contributiva]) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>(Sum((-Bonus / 13.5) - (-Bonus * 0.005)) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>(Sum(-[Rateo INAIL]) * [Maternità Facoltativa])</t>
-  </si>
-  <si>
-    <t>(Sum(-[RAL] / 26 * [Ferie Godute]))</t>
-  </si>
-  <si>
-    <t>(Sum(-[RAL] / 26 * [Ferie Godute] * [Aliquota Contributiva]))</t>
-  </si>
-  <si>
-    <t>(Sum(RangeSum(-[Retribuzione Lorda] , -(([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]))) * [Cessato])</t>
-  </si>
-  <si>
-    <t>(Sum(-Straordinario) * [Cessato])</t>
-  </si>
-  <si>
-    <t>(Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità])) * [Cessato])</t>
-  </si>
-  <si>
-    <t>(Sum(-[Rateo Ferie e Festività]) * [Cessato])</t>
-  </si>
-  <si>
-    <t>(Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])))) * [Cessato])</t>
-  </si>
-  <si>
-    <t>(Sum(-Straordinario * [Aliquota Contributiva])* [Cessato])</t>
-  </si>
-  <si>
-    <t>(Sum(-Bonus) * [Cessato])</t>
-  </si>
-  <si>
-    <t>(Sum(-Bonus * [Aliquota Contributiva]) * [Cessato])</t>
-  </si>
-  <si>
-    <t>(Sum((-Bonus / 13.5) - (-Bonus * 0.005)) * [Cessato])</t>
-  </si>
-  <si>
-    <t>(Sum(-[Contributi su Ratei]) * [Cessato])</t>
-  </si>
-  <si>
-    <t>(Sum(-[Rateo TFR]) * [Cessato])</t>
-  </si>
-  <si>
-    <t>(Sum(-[Rateo INAIL]) * [Cessato])</t>
-  </si>
-  <si>
-    <t>(Sum([Retribuzione Lorda])
+)) * Alt([Maternità], 0), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(Aumento), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(Aumento) / 6, '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum([Aumento] * [Rateo Ferie e Festività] / [RAL]), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum([Aumento] * 0.0805864), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(RangeSum(-([RAL] * 0.8), - (([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]))) * Alt([Maternità], 0), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-Straordinario) * Alt([Maternità], 0), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-Straordinario * [Aliquota Contributiva]) * Alt([Maternità], 0), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(RangeSum(-[Retribuzione Lorda] , -(([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]))) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-Straordinario) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità])) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-[Rateo Ferie e Festività]) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])))) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-Straordinario * [Aliquota Contributiva]) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità], -[Rateo Ferie e Festività]) * [Aliquota Contributiva]) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-Bonus) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-Bonus * [Aliquota Contributiva]) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum((-Bonus / 13.5) - (-Bonus * 0.005)) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-[Rateo INAIL]) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-[RAL] / 26 * [Ferie Godute]), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-[RAL] / 26 * [Ferie Godute] * [Aliquota Contributiva]), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(RangeSum(-[Retribuzione Lorda] , -(([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]))) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-Straordinario) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità])) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-[Rateo Ferie e Festività]) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])))) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-Straordinario * [Aliquota Contributiva])* [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-Bonus) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-Bonus * [Aliquota Contributiva]) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum((-Bonus / 13.5) - (-Bonus * 0.005)) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-[Contributi su Ratei]) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-[Rateo TFR]) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-[Rateo INAIL]) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum([Retribuzione Lorda])
   + Sum([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]
   + Sum(Bonus)
   + Sum(Straordinario)
@@ -595,7 +577,25 @@
   + (Sum(-[Contributi su Ratei]) * [Cessato])
   + (Sum(-[Rateo TFR]) * [Cessato])
   + (Sum(-[Rateo INAIL]) * [Cessato])
- )</t>
+ , '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum([Retribuzione Lorda])
+  + Sum([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]
+  + Sum(Bonus)
+  + Sum(Straordinario)
+  + Sum([Contributi su Retribuzione])
+  + Sum(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva]))
+  + Sum(Bonus * [Aliquota Contributiva])
+  + Sum(Straordinario * [Aliquota Contributiva])
+  + Sum([Rateo 13ª Mensilità])
+  + Sum([Rateo 14ª Mensilità])
+  + Sum([Rateo Ferie e Festività])
+  + Sum([Rateo TFR])
+  + Sum((Bonus / 13.5) - (Bonus * 0.005))
+  + Sum([Rateo INAIL])
+  + Sum([Contributi su Ratei])
+ , '#.##0,00')</t>
   </si>
 </sst>
 </file>
@@ -665,7 +665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -697,9 +697,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -997,30 +994,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="52.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="128.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="96.140625" style="2" customWidth="1"/>
     <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1035,7 +1032,7 @@
         <v>17</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1049,7 +1046,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1063,7 +1060,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1077,7 +1074,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1091,7 +1088,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1259,7 +1256,7 @@
         <v>19</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>124</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1315,7 +1312,7 @@
         <v>20</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1329,7 +1326,7 @@
         <v>21</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1343,7 +1340,7 @@
         <v>22</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1357,7 +1354,7 @@
         <v>23</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1371,7 +1368,7 @@
         <v>24</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="72">
@@ -1385,10 +1382,10 @@
         <v>25</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="24">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1427,7 +1424,7 @@
         <v>43</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1441,7 +1438,7 @@
         <v>44</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1455,7 +1452,7 @@
         <v>45</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1469,7 +1466,7 @@
         <v>46</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1483,7 +1480,7 @@
         <v>47</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1497,7 +1494,7 @@
         <v>29</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1511,7 +1508,7 @@
         <v>48</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1525,7 +1522,7 @@
         <v>49</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1539,7 +1536,7 @@
         <v>50</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1553,7 +1550,7 @@
         <v>51</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1567,7 +1564,7 @@
         <v>52</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1581,7 +1578,7 @@
         <v>53</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1595,7 +1592,7 @@
         <v>54</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1623,7 +1620,7 @@
         <v>30</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1637,7 +1634,7 @@
         <v>31</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1651,7 +1648,7 @@
         <v>56</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1665,7 +1662,7 @@
         <v>57</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1679,7 +1676,7 @@
         <v>55</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1693,7 +1690,7 @@
         <v>32</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1707,7 +1704,7 @@
         <v>60</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1721,7 +1718,7 @@
         <v>59</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1735,7 +1732,7 @@
         <v>33</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1749,7 +1746,7 @@
         <v>35</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1763,7 +1760,7 @@
         <v>37</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1777,7 +1774,7 @@
         <v>34</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1791,7 +1788,7 @@
         <v>36</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1805,7 +1802,7 @@
         <v>58</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="99.95" customHeight="1">
@@ -1819,7 +1816,7 @@
         <v>26</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E58" s="4"/>
     </row>

</xml_diff>

<commit_message>
Sostituito il valore 5,29 con 6 per azzerare temporaneamente i contributi su ticket prima di una modifica che tenga conto del diverso limite di contribuzione per i ticket elettronici o cartacei
</commit_message>
<xml_diff>
--- a/BudgetHR/Local/License/Lyreco/Excel/Conti.xlsx
+++ b/BudgetHR/Local/License/Lyreco/Excel/Conti.xlsx
@@ -362,9 +362,6 @@
     <t>Num(Sum([Contributi su Retribuzione]), '#.##0,00')</t>
   </si>
   <si>
-    <t>Num(Sum(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])), '#.##0,00')</t>
-  </si>
-  <si>
     <t>Num(Sum(Bonus * [Aliquota Contributiva]), '#.##0,00')</t>
   </si>
   <si>
@@ -390,6 +387,125 @@
   </si>
   <si>
     <t>Num(Sum([Contributi su Ratei]), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(
+  (Aumento 
+  + (Aumento / 6)
+  + ([Aumento] * [Rateo Ferie e Festività] / [RAL])
+  ) * [Aliquota Contributiva]
+ ), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(Aumento), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(Aumento) / 6, '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum([Aumento] * [Rateo Ferie e Festività] / [RAL]), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum([Aumento] * 0.0805864), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(RangeSum(-([RAL] * 0.8), - (([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]))) * Alt([Maternità], 0), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-Straordinario) * Alt([Maternità], 0), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-Straordinario * [Aliquota Contributiva]) * Alt([Maternità], 0), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(RangeSum(-[Retribuzione Lorda] , -(([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]))) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-Straordinario) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità])) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-[Rateo Ferie e Festività]) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-Straordinario * [Aliquota Contributiva]) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità], -[Rateo Ferie e Festività]) * [Aliquota Contributiva]) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-Bonus) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-Bonus * [Aliquota Contributiva]) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum((-Bonus / 13.5) - (-Bonus * 0.005)) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-[Rateo INAIL]) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-[RAL] / 26 * [Ferie Godute]), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-[RAL] / 26 * [Ferie Godute] * [Aliquota Contributiva]), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(RangeSum(-[Retribuzione Lorda] , -(([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]))) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-Straordinario) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità])) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-[Rateo Ferie e Festività]) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-Straordinario * [Aliquota Contributiva])* [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-Bonus) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-Bonus * [Aliquota Contributiva]) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum((-Bonus / 13.5) - (-Bonus * 0.005)) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-[Contributi su Ratei]) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-[Rateo TFR]) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(-[Rateo INAIL]) * [Cessato], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 6) * [Aliquota Contributiva])), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum([Retribuzione Lorda])
+  + Sum([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]
+  + Sum(Bonus)
+  + Sum(Straordinario)
+  + Sum([Contributi su Retribuzione])
+  + Sum(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 6) * [Aliquota Contributiva]))
+  + Sum(Bonus * [Aliquota Contributiva])
+  + Sum(Straordinario * [Aliquota Contributiva])
+  + Sum([Rateo 13ª Mensilità])
+  + Sum([Rateo 14ª Mensilità])
+  + Sum([Rateo Ferie e Festività])
+  + Sum([Rateo TFR])
+  + Sum((Bonus / 13.5) - (Bonus * 0.005))
+  + Sum([Rateo INAIL])
+  + Sum([Contributi su Ratei])
+ , '#.##0,00')</t>
   </si>
   <si>
     <t>Num((Sum([Retribuzione Lorda])
@@ -397,7 +513,7 @@
   + Sum(Bonus)
   + Sum(Straordinario)
   + Sum([Contributi su Retribuzione])
-  + Sum(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva]))
+  + Sum(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 6) * [Aliquota Contributiva]))
   + Sum(Bonus * [Aliquota Contributiva])
   + Sum(Straordinario * [Aliquota Contributiva])
   + Sum([Rateo 13ª Mensilità])
@@ -410,114 +526,16 @@
   ) / (Sum([Ore Lavoro Ordinario]) + Sum([Ore Lavoro Straordinario]) + Sum([Straordinario] / (([RAL] / 168) * [Maggiorazione Straordinario]))), '#.##0,00')</t>
   </si>
   <si>
-    <t>Num(Sum(
-  (Aumento 
-  + (Aumento / 6)
-  + ([Aumento] * [Rateo Ferie e Festività] / [RAL])
-  ) * [Aliquota Contributiva]
- ), '#.##0,00')</t>
-  </si>
-  <si>
     <t>Num(Sum(RangeSum(
  - ([RAL] * 0.8 * [Aliquota Contributiva])
- - ((([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])))
+ - ((([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 6) * [Aliquota Contributiva])))
 )) * Alt([Maternità], 0), '#.##0,00')</t>
   </si>
   <si>
-    <t>Num(Sum(Aumento), '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(Aumento) / 6, '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum([Aumento] * [Rateo Ferie e Festività] / [RAL]), '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum([Aumento] * 0.0805864), '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(RangeSum(-([RAL] * 0.8), - (([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]))) * Alt([Maternità], 0), '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(-Straordinario) * Alt([Maternità], 0), '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(-Straordinario * [Aliquota Contributiva]) * Alt([Maternità], 0), '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(RangeSum(-[Retribuzione Lorda] , -(([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]))) * [Maternità Facoltativa], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(-Straordinario) * [Maternità Facoltativa], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità])) * [Maternità Facoltativa], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(-[Rateo Ferie e Festività]) * [Maternità Facoltativa], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])))) * [Maternità Facoltativa], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(-Straordinario * [Aliquota Contributiva]) * [Maternità Facoltativa], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità], -[Rateo Ferie e Festività]) * [Aliquota Contributiva]) * [Maternità Facoltativa], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(-Bonus) * [Maternità Facoltativa], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(-Bonus * [Aliquota Contributiva]) * [Maternità Facoltativa], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum((-Bonus / 13.5) - (-Bonus * 0.005)) * [Maternità Facoltativa], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(-[Rateo INAIL]) * [Maternità Facoltativa], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(-[RAL] / 26 * [Ferie Godute]), '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(-[RAL] / 26 * [Ferie Godute] * [Aliquota Contributiva]), '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(RangeSum(-[Retribuzione Lorda] , -(([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]))) * [Cessato], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(-Straordinario) * [Cessato], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità])) * [Cessato], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(-[Rateo Ferie e Festività]) * [Cessato], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])))) * [Cessato], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(-Straordinario * [Aliquota Contributiva])* [Cessato], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(-Bonus) * [Cessato], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(-Bonus * [Aliquota Contributiva]) * [Cessato], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum((-Bonus / 13.5) - (-Bonus * 0.005)) * [Cessato], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(-[Contributi su Ratei]) * [Cessato], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(-[Rateo TFR]) * [Cessato], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(-[Rateo INAIL]) * [Cessato], '#.##0,00')</t>
+    <t>Num(Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 6) * [Aliquota Contributiva])))) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 6) * [Aliquota Contributiva])))) * [Cessato], '#.##0,00')</t>
   </si>
   <si>
     <t>Num(Sum([Retribuzione Lorda])
@@ -525,7 +543,7 @@
   + Sum(Bonus)
   + Sum(Straordinario)
   + Sum([Contributi su Retribuzione])
-  + Sum(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva]))
+  + Sum(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 6) * [Aliquota Contributiva]))
   + Sum(Bonus * [Aliquota Contributiva])
   + Sum(Straordinario * [Aliquota Contributiva])
   + Sum([Rateo 13ª Mensilità])
@@ -549,14 +567,14 @@
   + (Sum(-Straordinario) * Alt([Maternità], 0))
   + (Sum(RangeSum(
    - ([RAL] * 0.8 * [Aliquota Contributiva])
-   - ((([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])))
+   - ((([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 6) * [Aliquota Contributiva])))
   )) * Alt([Maternità], 0))
   + (Sum(-Straordinario * [Aliquota Contributiva]) * Alt([Maternità], 0))
   + (Sum(RangeSum(-[Retribuzione Lorda] , -(([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]))) * [Maternità Facoltativa])
   + (Sum(-Straordinario) * [Maternità Facoltativa])
   + (Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità])) * [Maternità Facoltativa])
   + (Sum(-[Rateo Ferie e Festività]) * [Maternità Facoltativa])
-  + (Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])))) * [Maternità Facoltativa])
+  + (Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 6) * [Aliquota Contributiva])))) * [Maternità Facoltativa])
   + (Sum(-Straordinario * [Aliquota Contributiva]) * [Maternità Facoltativa])
   + (Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità], -[Rateo Ferie e Festività]) * [Aliquota Contributiva]) * [Maternità Facoltativa])
   + (Sum(-Bonus) * [Maternità Facoltativa])
@@ -569,7 +587,7 @@
   + (Sum(-Straordinario) * [Cessato])
   + (Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità])) * [Cessato])
   + (Sum(-[Rateo Ferie e Festività]) * [Cessato])
-  + (Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva])))) * [Cessato])
+  + (Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 6) * [Aliquota Contributiva])))) * [Cessato])
   + (Sum(-Straordinario * [Aliquota Contributiva]) * [Cessato])
   + (Sum(-Bonus) * [Cessato])
   + (Sum(-Bonus * [Aliquota Contributiva]) * [Cessato])
@@ -577,24 +595,6 @@
   + (Sum(-[Contributi su Ratei]) * [Cessato])
   + (Sum(-[Rateo TFR]) * [Cessato])
   + (Sum(-[Rateo INAIL]) * [Cessato])
- , '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum([Retribuzione Lorda])
-  + Sum([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]
-  + Sum(Bonus)
-  + Sum(Straordinario)
-  + Sum([Contributi su Retribuzione])
-  + Sum(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 5.29) * [Aliquota Contributiva]))
-  + Sum(Bonus * [Aliquota Contributiva])
-  + Sum(Straordinario * [Aliquota Contributiva])
-  + Sum([Rateo 13ª Mensilità])
-  + Sum([Rateo 14ª Mensilità])
-  + Sum([Rateo Ferie e Festività])
-  + Sum([Rateo TFR])
-  + Sum((Bonus / 13.5) - (Bonus * 0.005))
-  + Sum([Rateo INAIL])
-  + Sum([Contributi su Ratei])
  , '#.##0,00')</t>
   </si>
 </sst>
@@ -994,7 +994,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -1116,7 +1116,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>114</v>
+        <v>154</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1130,7 +1130,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1144,7 +1144,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1158,7 +1158,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1172,7 +1172,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1186,7 +1186,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1200,7 +1200,7 @@
         <v>4</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1214,7 +1214,7 @@
         <v>18</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1228,7 +1228,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1242,7 +1242,7 @@
         <v>16</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="60" customHeight="1">
@@ -1256,7 +1256,7 @@
         <v>19</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1312,7 +1312,7 @@
         <v>20</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>124</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1326,7 +1326,7 @@
         <v>21</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1340,7 +1340,7 @@
         <v>22</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1354,7 +1354,7 @@
         <v>23</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1368,7 +1368,7 @@
         <v>24</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="72">
@@ -1382,7 +1382,7 @@
         <v>25</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="24">
@@ -1396,7 +1396,7 @@
         <v>41</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1410,7 +1410,7 @@
         <v>42</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="48">
@@ -1424,7 +1424,7 @@
         <v>43</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>126</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1438,7 +1438,7 @@
         <v>44</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1452,7 +1452,7 @@
         <v>45</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1466,7 +1466,7 @@
         <v>46</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1480,7 +1480,7 @@
         <v>47</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1494,7 +1494,7 @@
         <v>29</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1508,7 +1508,7 @@
         <v>48</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1522,7 +1522,7 @@
         <v>49</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1536,7 +1536,7 @@
         <v>50</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1550,7 +1550,7 @@
         <v>51</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1564,7 +1564,7 @@
         <v>52</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1578,7 +1578,7 @@
         <v>53</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1592,7 +1592,7 @@
         <v>54</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:4">
@@ -1620,7 +1620,7 @@
         <v>30</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1634,7 +1634,7 @@
         <v>31</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1648,7 +1648,7 @@
         <v>56</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1662,7 +1662,7 @@
         <v>57</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1676,7 +1676,7 @@
         <v>55</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1690,7 +1690,7 @@
         <v>32</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1704,7 +1704,7 @@
         <v>60</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1718,7 +1718,7 @@
         <v>59</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1732,7 +1732,7 @@
         <v>33</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1746,7 +1746,7 @@
         <v>35</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1760,7 +1760,7 @@
         <v>37</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1774,7 +1774,7 @@
         <v>34</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1788,7 +1788,7 @@
         <v>36</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1802,7 +1802,7 @@
         <v>58</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="99.95" customHeight="1">
@@ -1816,7 +1816,7 @@
         <v>26</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E58" s="4"/>
     </row>

</xml_diff>

<commit_message>
Agginta Deducibilità variabile del ticket, € 5,29 e € 7,00 Suddivisione dei Contributi su Ratei in Contributi su 13 e 14 mensilità e Contributi su Ferie e Festività
</commit_message>
<xml_diff>
--- a/BudgetHR/Local/License/Lyreco/Excel/Conti.xlsx
+++ b/BudgetHR/Local/License/Lyreco/Excel/Conti.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="163">
   <si>
     <t>Rateo 13ª Mensilità</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Contributi su Straordinario</t>
-  </si>
-  <si>
-    <t>Contributi su Ratei</t>
   </si>
   <si>
     <t>RAL</t>
@@ -384,9 +381,6 @@
   </si>
   <si>
     <t>Num(Sum([Rateo INAIL]), '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum([Contributi su Ratei]), '#.##0,00')</t>
   </si>
   <si>
     <t>Num(Sum(
@@ -487,7 +481,19 @@
     <t>Num(Sum(-[Rateo INAIL]) * [Cessato], '#.##0,00')</t>
   </si>
   <si>
-    <t>Num(Sum(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 6) * [Aliquota Contributiva])), '#.##0,00')</t>
+    <t>Contributi su Ferie e Festività</t>
+  </si>
+  <si>
+    <t>Contributi su 13ª e 14ª Mensilità</t>
+  </si>
+  <si>
+    <t>Num(Sum([Contributi su 13ª e 14ª Mensilità]), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum([Contributi su Ferie e Festività]), '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(([GG Lavorativi] - [Ferie Godute]) * (RangeMax([Valore Ticket] - $(App.GetValoreDeducibilitàTicket), 0) * [Aliquota Contributiva])), '#.##0,00')</t>
   </si>
   <si>
     <t>Num(Sum([Retribuzione Lorda])
@@ -495,7 +501,7 @@
   + Sum(Bonus)
   + Sum(Straordinario)
   + Sum([Contributi su Retribuzione])
-  + Sum(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 6) * [Aliquota Contributiva]))
+  + Sum(([GG Lavorativi] - [Ferie Godute]) * (RangeMax([Valore Ticket] - $(App.GetValoreDeducibilitàTicket), 0) * [Aliquota Contributiva]))
   + Sum(Bonus * [Aliquota Contributiva])
   + Sum(Straordinario * [Aliquota Contributiva])
   + Sum([Rateo 13ª Mensilità])
@@ -513,7 +519,7 @@
   + Sum(Bonus)
   + Sum(Straordinario)
   + Sum([Contributi su Retribuzione])
-  + Sum(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 6) * [Aliquota Contributiva]))
+  + Sum(([GG Lavorativi] - [Ferie Godute]) * (RangeMax([Valore Ticket] - $(App.GetValoreDeducibilitàTicket), 0) * [Aliquota Contributiva]))
   + Sum(Bonus * [Aliquota Contributiva])
   + Sum(Straordinario * [Aliquota Contributiva])
   + Sum([Rateo 13ª Mensilità])
@@ -528,14 +534,14 @@
   <si>
     <t>Num(Sum(RangeSum(
  - ([RAL] * 0.8 * [Aliquota Contributiva])
- - ((([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 6) * [Aliquota Contributiva])))
+ - ((([GG Lavorativi] - [Ferie Godute]) * (RangeMax([Valore Ticket] - $(App.GetValoreDeducibilitàTicket), 0) * [Aliquota Contributiva])))
 )) * Alt([Maternità], 0), '#.##0,00')</t>
   </si>
   <si>
-    <t>Num(Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 6) * [Aliquota Contributiva])))) * [Maternità Facoltativa], '#.##0,00')</t>
-  </si>
-  <si>
-    <t>Num(Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 6) * [Aliquota Contributiva])))) * [Cessato], '#.##0,00')</t>
+    <t>Num(Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (RangeMax([Valore Ticket] - $(App.GetValoreDeducibilitàTicket), 0) * [Aliquota Contributiva])))) * [Maternità Facoltativa], '#.##0,00')</t>
+  </si>
+  <si>
+    <t>Num(Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (RangeMax([Valore Ticket] - $(App.GetValoreDeducibilitàTicket), 0) * [Aliquota Contributiva])))) * [Cessato], '#.##0,00')</t>
   </si>
   <si>
     <t>Num(Sum([Retribuzione Lorda])
@@ -543,7 +549,7 @@
   + Sum(Bonus)
   + Sum(Straordinario)
   + Sum([Contributi su Retribuzione])
-  + Sum(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 6) * [Aliquota Contributiva]))
+  + Sum(([GG Lavorativi] - [Ferie Godute]) * (RangeMax([Valore Ticket] - $(App.GetValoreDeducibilitàTicket), 0) * [Aliquota Contributiva]))
   + Sum(Bonus * [Aliquota Contributiva])
   + Sum(Straordinario * [Aliquota Contributiva])
   + Sum([Rateo 13ª Mensilità])
@@ -567,14 +573,14 @@
   + (Sum(-Straordinario) * Alt([Maternità], 0))
   + (Sum(RangeSum(
    - ([RAL] * 0.8 * [Aliquota Contributiva])
-   - ((([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 6) * [Aliquota Contributiva])))
+   - ((([GG Lavorativi] - [Ferie Godute]) * (RangeMax([Valore Ticket] - $(App.GetValoreDeducibilitàTicket), 0) * [Aliquota Contributiva])))
   )) * Alt([Maternità], 0))
   + (Sum(-Straordinario * [Aliquota Contributiva]) * Alt([Maternità], 0))
   + (Sum(RangeSum(-[Retribuzione Lorda] , -(([GG Lavorativi] - [Ferie Godute]) * [Valore Ticket]))) * [Maternità Facoltativa])
   + (Sum(-Straordinario) * [Maternità Facoltativa])
   + (Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità])) * [Maternità Facoltativa])
   + (Sum(-[Rateo Ferie e Festività]) * [Maternità Facoltativa])
-  + (Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 6) * [Aliquota Contributiva])))) * [Maternità Facoltativa])
+  + (Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (RangeMax([Valore Ticket] - $(App.GetValoreDeducibilitàTicket), 0) * [Aliquota Contributiva])))) * [Maternità Facoltativa])
   + (Sum(-Straordinario * [Aliquota Contributiva]) * [Maternità Facoltativa])
   + (Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità], -[Rateo Ferie e Festività]) * [Aliquota Contributiva]) * [Maternità Facoltativa])
   + (Sum(-Bonus) * [Maternità Facoltativa])
@@ -587,7 +593,7 @@
   + (Sum(-Straordinario) * [Cessato])
   + (Sum(RangeSum(-[Rateo 13ª Mensilità], -[Rateo 14ª Mensilità])) * [Cessato])
   + (Sum(-[Rateo Ferie e Festività]) * [Cessato])
-  + (Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (([Valore Ticket] - 6) * [Aliquota Contributiva])))) * [Cessato])
+  + (Sum(RangeSum(-[Contributi su Retribuzione], -(([GG Lavorativi] - [Ferie Godute]) * (RangeMax([Valore Ticket] - $(App.GetValoreDeducibilitàTicket), 0) * [Aliquota Contributiva])))) * [Cessato])
   + (Sum(-Straordinario * [Aliquota Contributiva]) * [Cessato])
   + (Sum(-Bonus) * [Cessato])
   + (Sum(-Bonus * [Aliquota Contributiva]) * [Cessato])
@@ -992,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12"/>
@@ -1009,16 +1015,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1026,13 +1032,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1046,7 +1052,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1060,7 +1066,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1074,7 +1080,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1088,7 +1094,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1102,10 +1108,10 @@
         <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="24">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1116,7 +1122,7 @@
         <v>13</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1130,7 +1136,7 @@
         <v>14</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1144,7 +1150,7 @@
         <v>15</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1158,7 +1164,7 @@
         <v>0</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1172,7 +1178,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1186,7 +1192,7 @@
         <v>2</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1200,7 +1206,7 @@
         <v>4</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1211,10 +1217,10 @@
         <v>140402</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1228,7 +1234,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1239,38 +1245,38 @@
         <v>143012</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>16</v>
+        <v>153</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="60" customHeight="1">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="2">
         <v>17</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>98</v>
+      <c r="B18" s="2">
+        <v>444444</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" ht="60" customHeight="1">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>39</v>
+        <v>18</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1278,13 +1284,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1292,41 +1298,41 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="76.5" customHeight="1">
+        <v>6</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>93</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="76.5" customHeight="1">
       <c r="A23" s="2">
         <v>22</v>
       </c>
-      <c r="B23" s="2">
-        <v>140001</v>
+      <c r="B23" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>124</v>
+        <v>19</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1334,13 +1340,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="2">
-        <v>140003</v>
+        <v>140001</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1348,13 +1354,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="2">
-        <v>141402</v>
+        <v>140003</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>126</v>
+        <v>21</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1362,72 +1368,72 @@
         <v>25</v>
       </c>
       <c r="B26" s="2">
-        <v>140402</v>
+        <v>141402</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="72">
+        <v>22</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="B27" s="2">
-        <v>143001</v>
+        <v>140402</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="24">
+        <v>23</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="72">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="B28" s="2">
-        <v>140001</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>41</v>
+        <v>143001</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="24">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="B29" s="2">
-        <v>140301</v>
+        <v>140001</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="48">
+        <v>40</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="B30" s="2">
-        <v>143001</v>
+        <v>140301</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>41</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="60">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1435,10 +1441,10 @@
         <v>143001</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>130</v>
+        <v>42</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1446,13 +1452,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="2">
-        <v>140001</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>45</v>
+        <v>143001</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -1460,13 +1466,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="2">
-        <v>140301</v>
+        <v>140001</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -1474,13 +1480,13 @@
         <v>33</v>
       </c>
       <c r="B34" s="2">
-        <v>140003</v>
+        <v>140301</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1488,13 +1494,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="2">
-        <v>141402</v>
+        <v>140003</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -1502,13 +1508,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="2">
-        <v>143001</v>
+        <v>141402</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -1519,10 +1525,10 @@
         <v>143001</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1530,13 +1536,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="2">
-        <v>143012</v>
+        <v>143001</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -1544,13 +1550,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="2">
-        <v>140201</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>51</v>
+        <v>143012</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:4">
@@ -1558,13 +1564,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="2">
-        <v>143001</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>52</v>
+        <v>140201</v>
+      </c>
+      <c r="C40" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:4">
@@ -1572,13 +1578,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="2">
-        <v>140402</v>
+        <v>143001</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:4">
@@ -1586,41 +1592,41 @@
         <v>41</v>
       </c>
       <c r="B42" s="2">
-        <v>143002</v>
+        <v>140402</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="2">
         <v>42</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>96</v>
+      <c r="B43" s="2">
+        <v>143002</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>97</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="2">
         <v>43</v>
       </c>
-      <c r="B44" s="2">
-        <v>141402</v>
+      <c r="B44" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>30</v>
+        <v>95</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>141</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" spans="1:4">
@@ -1628,13 +1634,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="2">
-        <v>143012</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>31</v>
+        <v>141402</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>29</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:4">
@@ -1642,13 +1648,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="2">
-        <v>140001</v>
+        <v>143012</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="1:4">
@@ -1656,13 +1662,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="2">
-        <v>140301</v>
+        <v>140001</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -1670,13 +1676,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="2">
-        <v>140003</v>
+        <v>140301</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1684,13 +1690,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="2">
-        <v>141402</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>32</v>
+        <v>140003</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1698,13 +1704,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="2">
-        <v>143001</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>60</v>
+        <v>141402</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1718,7 +1724,7 @@
         <v>59</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>147</v>
+        <v>161</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1726,13 +1732,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="2">
-        <v>140201</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>33</v>
+        <v>143001</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1740,13 +1746,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="2">
-        <v>143001</v>
+        <v>140201</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1754,13 +1760,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="2">
-        <v>140402</v>
+        <v>143001</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1768,13 +1774,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="2">
-        <v>143012</v>
+        <v>140402</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1782,13 +1788,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="2">
-        <v>140402</v>
+        <v>143012</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1796,29 +1802,43 @@
         <v>56</v>
       </c>
       <c r="B57" s="2">
-        <v>143002</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>58</v>
+        <v>140402</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="99.95" customHeight="1">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" s="2">
         <v>57</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>104</v>
+      <c r="B58" s="2">
+        <v>143002</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>160</v>
-      </c>
-      <c r="E58" s="4"/>
+        <v>57</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="99.95" customHeight="1">
+      <c r="A59" s="2">
+        <v>58</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E59" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1844,13 +1864,13 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1858,10 +1878,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -1869,10 +1889,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -1880,10 +1900,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1891,10 +1911,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -1902,10 +1922,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1913,10 +1933,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1924,10 +1944,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="60">
@@ -1935,10 +1955,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>106</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1946,10 +1966,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1957,10 +1977,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1968,10 +1988,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1979,10 +1999,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1990,10 +2010,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2001,10 +2021,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2012,10 +2032,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2023,10 +2043,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>